<commit_message>
testAdjacenciesInsideRoom method protrays actual board cell values with relation to the excel file:
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="31">
   <si>
     <t xml:space="preserve">K</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">S</t>
   </si>
   <si>
+    <t xml:space="preserve">KR</t>
+  </si>
+  <si>
     <t xml:space="preserve">KD</t>
   </si>
   <si>
@@ -91,7 +94,7 @@
     <t xml:space="preserve">BL</t>
   </si>
   <si>
-    <t xml:space="preserve">Number of doors: 11</t>
+    <t xml:space="preserve">Number of doors: 15</t>
   </si>
   <si>
     <t xml:space="preserve">White: door direction tests</t>
@@ -379,8 +382,8 @@
   </sheetPr>
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D34" activeCellId="0" sqref="D34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P34" activeCellId="0" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -544,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>1</v>
@@ -612,7 +615,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -763,10 +766,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>1</v>
@@ -775,13 +778,13 @@
         <v>3</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>3</v>
@@ -816,14 +819,14 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -885,16 +888,16 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>1</v>
@@ -939,16 +942,16 @@
         <v>1</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="U8" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="U8" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="V8" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W8" s="0" t="n">
         <v>7</v>
@@ -956,16 +959,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>1</v>
@@ -974,19 +977,19 @@
         <v>1</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>1</v>
@@ -1010,16 +1013,16 @@
         <v>1</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W9" s="0" t="n">
         <v>8</v>
@@ -1027,16 +1030,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1</v>
@@ -1045,19 +1048,19 @@
         <v>1</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K10" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>1</v>
@@ -1065,32 +1068,32 @@
       <c r="M10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>16</v>
+      <c r="N10" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W10" s="0" t="n">
         <v>9</v>
@@ -1098,16 +1101,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1</v>
@@ -1116,19 +1119,19 @@
         <v>1</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>1</v>
@@ -1137,31 +1140,31 @@
         <v>1</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W11" s="0" t="n">
         <v>10</v>
@@ -1169,16 +1172,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>1</v>
@@ -1187,19 +1190,19 @@
         <v>1</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K12" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>1</v>
@@ -1208,31 +1211,31 @@
         <v>1</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W12" s="0" t="n">
         <v>11</v>
@@ -1240,16 +1243,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>1</v>
@@ -1258,19 +1261,19 @@
         <v>1</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H13" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J13" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K13" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>1</v>
@@ -1279,31 +1282,31 @@
         <v>1</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>12</v>
@@ -1350,31 +1353,31 @@
         <v>1</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>13</v>
@@ -1421,31 +1424,31 @@
         <v>1</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="T15" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>14</v>
@@ -1453,13 +1456,13 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>1</v>
@@ -1468,19 +1471,19 @@
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>1</v>
@@ -1492,31 +1495,31 @@
         <v>1</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>15</v>
@@ -1524,13 +1527,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>1</v>
@@ -1539,19 +1542,19 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>1</v>
@@ -1563,31 +1566,31 @@
         <v>1</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>16</v>
@@ -1595,13 +1598,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>1</v>
@@ -1610,19 +1613,19 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>1</v>
@@ -1634,31 +1637,31 @@
         <v>1</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W18" s="0" t="n">
         <v>17</v>
@@ -1666,34 +1669,34 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>1</v>
@@ -1705,31 +1708,31 @@
         <v>1</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W19" s="0" t="n">
         <v>18</v>
@@ -1737,34 +1740,34 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>1</v>
@@ -1776,31 +1779,31 @@
         <v>1</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W20" s="0" t="n">
         <v>19</v>
@@ -1808,13 +1811,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>1</v>
@@ -1823,19 +1826,19 @@
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>1</v>
@@ -1847,31 +1850,31 @@
         <v>1</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="W21" s="0" t="n">
         <v>20</v>
@@ -1947,37 +1950,37 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the skeleton for testAdjacencyDoorways
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="30">
   <si>
     <t xml:space="preserve">K</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t xml:space="preserve">KR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">KD</t>
   </si>
   <si>
     <t xml:space="preserve">MD</t>
@@ -254,7 +251,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -279,7 +276,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -287,11 +288,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -382,8 +383,8 @@
   </sheetPr>
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P34" activeCellId="0" sqref="P34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>0</v>
@@ -685,10 +686,10 @@
       <c r="C5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -766,25 +767,25 @@
         <v>1</v>
       </c>
       <c r="G6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="I6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>10</v>
-      </c>
       <c r="L6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="M6" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="N6" s="2" t="s">
         <v>3</v>
@@ -819,14 +820,14 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>1</v>
@@ -834,7 +835,7 @@
       <c r="F7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="3" t="s">
@@ -888,70 +889,70 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="L8" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="S8" s="6" t="s">
+      <c r="T8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="T8" s="9" t="s">
-        <v>13</v>
-      </c>
       <c r="U8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W8" s="0" t="n">
         <v>7</v>
@@ -959,16 +960,16 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>1</v>
@@ -976,20 +977,20 @@
       <c r="F9" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>15</v>
+      <c r="G9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>1</v>
@@ -1013,16 +1014,16 @@
         <v>1</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W9" s="0" t="n">
         <v>8</v>
@@ -1030,16 +1031,16 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>1</v>
@@ -1047,20 +1048,20 @@
       <c r="F10" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J10" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>15</v>
+      <c r="G10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>1</v>
@@ -1069,31 +1070,31 @@
         <v>1</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W10" s="0" t="n">
         <v>9</v>
@@ -1101,16 +1102,16 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>1</v>
@@ -1118,20 +1119,20 @@
       <c r="F11" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>15</v>
+      <c r="G11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>1</v>
@@ -1140,31 +1141,31 @@
         <v>1</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W11" s="0" t="n">
         <v>10</v>
@@ -1172,16 +1173,16 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>1</v>
@@ -1189,20 +1190,20 @@
       <c r="F12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>15</v>
+      <c r="G12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>1</v>
@@ -1211,31 +1212,31 @@
         <v>1</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W12" s="0" t="n">
         <v>11</v>
@@ -1243,16 +1244,16 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>1</v>
@@ -1260,20 +1261,20 @@
       <c r="F13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J13" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>15</v>
+      <c r="G13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>14</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>1</v>
@@ -1282,31 +1283,31 @@
         <v>1</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W13" s="0" t="n">
         <v>12</v>
@@ -1353,31 +1354,31 @@
         <v>1</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W14" s="0" t="n">
         <v>13</v>
@@ -1405,7 +1406,7 @@
       <c r="G15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H15" s="7" t="s">
+      <c r="H15" s="8" t="s">
         <v>1</v>
       </c>
       <c r="I15" s="3" t="s">
@@ -1424,31 +1425,31 @@
         <v>1</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W15" s="0" t="n">
         <v>14</v>
@@ -1456,34 +1457,34 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="I16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>1</v>
@@ -1495,31 +1496,31 @@
         <v>1</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W16" s="0" t="n">
         <v>15</v>
@@ -1527,13 +1528,13 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>1</v>
@@ -1542,19 +1543,19 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>1</v>
@@ -1566,31 +1567,31 @@
         <v>1</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R17" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W17" s="0" t="n">
         <v>16</v>
@@ -1598,13 +1599,13 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>1</v>
@@ -1613,19 +1614,19 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>1</v>
@@ -1637,31 +1638,31 @@
         <v>1</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W18" s="0" t="n">
         <v>17</v>
@@ -1669,34 +1670,34 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>23</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>1</v>
@@ -1708,31 +1709,31 @@
         <v>1</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W19" s="0" t="n">
         <v>18</v>
@@ -1740,34 +1741,34 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K20" s="3" t="s">
         <v>1</v>
@@ -1779,31 +1780,31 @@
         <v>1</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W20" s="0" t="n">
         <v>19</v>
@@ -1811,13 +1812,13 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>1</v>
@@ -1826,19 +1827,19 @@
         <v>1</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K21" s="3" t="s">
         <v>1</v>
@@ -1850,31 +1851,31 @@
         <v>1</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>1</v>
       </c>
       <c r="S21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="W21" s="0" t="n">
         <v>20</v>
@@ -1950,37 +1951,37 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
switching this branch to failingAdjTests branch
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="30">
   <si>
     <t xml:space="preserve">K</t>
   </si>
@@ -383,8 +383,8 @@
   </sheetPr>
   <dimension ref="A1:W30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q27" activeCellId="0" sqref="Q27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G31" activeCellId="0" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -822,7 +822,9 @@
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="C7" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>